<commit_message>
update data extraction form
</commit_message>
<xml_diff>
--- a/data-raw/Data extraction form_FINAL.xlsx
+++ b/data-raw/Data extraction form_FINAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonahthomas/R_projects/gpad.cards/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA6BC95-39CC-9F4B-BA35-82FB29105245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A8DAB6-6DC5-1B4B-A7B6-45AB04D8ABD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{5BAB5DFC-CE5D-6E42-A4C3-D90D5449F9C0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15580" xr2:uid="{5BAB5DFC-CE5D-6E42-A4C3-D90D5449F9C0}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_extraction_form" sheetId="1" r:id="rId1"/>
@@ -2433,7 +2433,7 @@
   <dimension ref="A1:DF107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="U3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="V3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
@@ -21967,18 +21967,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22000,6 +22000,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4B90D25-620E-4D96-A051-F79F7073263B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14677FDD-19BE-416D-B404-BDD41C6725EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -22013,12 +22021,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4B90D25-620E-4D96-A051-F79F7073263B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>